<commit_message>
try to fix rest classification
</commit_message>
<xml_diff>
--- a/data/filenames-indexes_lpfilter.xlsx
+++ b/data/filenames-indexes_lpfilter.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikol/Desktop/engrCapst/ExoArm/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08C0891-CF47-B943-B13F-CFFFAD731B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D68DC64-7DA9-D944-8F01-FAFEF93B7843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>FILENAMES</t>
   </si>
@@ -42,18 +43,27 @@
   <si>
     <t>../data/lpdata/CoolTerm Capture 2023-03-28 10-41-00.txt</t>
   </si>
+  <si>
+    <t>../data/electrodeData/CoolTerm Capture 2023-03-28 15-39-11.txt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -70,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -93,13 +103,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -407,7 +435,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C10"/>
+      <selection activeCell="C4" sqref="C4:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -440,7 +468,7 @@
         <v>532</v>
       </c>
       <c r="C2">
-        <v>598</v>
+        <v>895</v>
       </c>
       <c r="E2">
         <v>2647</v>
@@ -454,7 +482,7 @@
         <v>763</v>
       </c>
       <c r="C3">
-        <v>895</v>
+        <v>1160</v>
       </c>
       <c r="E3">
         <v>2713</v>
@@ -465,7 +493,7 @@
         <v>1028</v>
       </c>
       <c r="C4">
-        <v>1160</v>
+        <v>2017</v>
       </c>
       <c r="E4">
         <v>2779</v>
@@ -476,7 +504,7 @@
         <v>1259</v>
       </c>
       <c r="C5">
-        <v>1391</v>
+        <v>2184</v>
       </c>
       <c r="E5">
         <v>2912</v>
@@ -487,7 +515,7 @@
         <v>1523</v>
       </c>
       <c r="C6">
-        <v>2017</v>
+        <v>2350</v>
       </c>
       <c r="E6">
         <v>2945</v>
@@ -498,7 +526,7 @@
         <v>1920</v>
       </c>
       <c r="C7">
-        <v>2184</v>
+        <v>2515</v>
       </c>
       <c r="E7">
         <v>2978</v>
@@ -509,7 +537,7 @@
         <v>2118</v>
       </c>
       <c r="C8">
-        <v>2350</v>
+        <v>3275</v>
       </c>
       <c r="E8">
         <v>3011</v>
@@ -519,9 +547,6 @@
       <c r="B9">
         <v>2284</v>
       </c>
-      <c r="C9">
-        <v>2515</v>
-      </c>
       <c r="E9">
         <v>3077</v>
       </c>
@@ -530,9 +555,6 @@
       <c r="B10">
         <v>2449</v>
       </c>
-      <c r="C10">
-        <v>3275</v>
-      </c>
       <c r="E10">
         <v>3143</v>
       </c>
@@ -540,6 +562,189 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>2812</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>668</v>
+      </c>
+      <c r="D2">
+        <v>767</v>
+      </c>
+      <c r="E2">
+        <v>1792</v>
+      </c>
+      <c r="F2">
+        <v>1990</v>
+      </c>
+      <c r="G2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>866</v>
+      </c>
+      <c r="D3">
+        <v>965</v>
+      </c>
+      <c r="E3">
+        <v>1891</v>
+      </c>
+      <c r="F3">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1064</v>
+      </c>
+      <c r="D4">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1263</v>
+      </c>
+      <c r="D5">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1527</v>
+      </c>
+      <c r="D6">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>2188</v>
+      </c>
+      <c r="D7">
+        <v>2287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>2386</v>
+      </c>
+      <c r="D8">
+        <v>2486</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>